<commit_message>
trie basic ops implemented
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447D27B9-4E2E-4F33-A01F-77BE181B61F3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4583764F-D958-4F9A-97F3-3F8B8471CA26}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1509,14 +1509,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFAFD095"/>
-        <bgColor rgb="FFC5E0B4"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFC5E0B4"/>
       </patternFill>
     </fill>
   </fills>
@@ -1944,8 +1944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A341" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B350" sqref="B350"/>
+    <sheetView tabSelected="1" topLeftCell="A335" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B355" sqref="B355"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
@@ -5578,7 +5578,7 @@
       <c r="A346" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="B346" s="14" t="s">
+      <c r="B346" s="13" t="s">
         <v>336</v>
       </c>
       <c r="C346" s="5" t="s">
@@ -5589,7 +5589,7 @@
       <c r="A347" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="B347" s="13" t="s">
+      <c r="B347" s="14" t="s">
         <v>337</v>
       </c>
       <c r="C347" s="5" t="s">
@@ -5622,7 +5622,7 @@
       <c r="A350" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="B350" s="7" t="s">
+      <c r="B350" s="13" t="s">
         <v>340</v>
       </c>
       <c r="C350" s="5" t="s">

</xml_diff>

<commit_message>
Sorting of stack added
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4BB74C-7A4A-4E82-9F0A-EFE0CDF374DD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6740FA7C-7E75-42B7-B582-74DADE806723}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1533,7 +1533,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1559,6 +1559,9 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1944,8 +1947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A297" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B305" sqref="B305"/>
+    <sheetView tabSelected="1" topLeftCell="A301" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B309" sqref="B309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
@@ -5185,7 +5188,7 @@
       <c r="A309" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="B309" s="11" t="s">
+      <c r="B309" s="15" t="s">
         <v>300</v>
       </c>
       <c r="C309" s="5" t="s">
@@ -5196,7 +5199,7 @@
       <c r="A310" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="B310" s="7" t="s">
+      <c r="B310" s="13" t="s">
         <v>301</v>
       </c>
       <c r="C310" s="5" t="s">
@@ -5240,7 +5243,7 @@
       <c r="A314" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="B314" s="7" t="s">
+      <c r="B314" s="13" t="s">
         <v>305</v>
       </c>
       <c r="C314" s="5" t="s">

</xml_diff>